<commit_message>
Added Database and tempCodeRunner to gitignore
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A2:XFD6"/>
@@ -465,27 +465,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LR33TEE</t>
+          <t>Z00MN65</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44084.20298954209</v>
+        <v>44084.54782234977</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44084.45189281521</v>
+        <v>44084.55539790984</v>
       </c>
       <c r="D2" t="n">
-        <v>358.4207132666667</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LR33TEE</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>44084.45253839267</v>
+        <v>10.9088065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add display of time entered, out and time spent
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -472,10 +472,10 @@
         <v>44084.54782234977</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44084.55539790984</v>
+        <v>44084.74785467862</v>
       </c>
       <c r="D2" t="n">
-        <v>10.9088065</v>
+        <v>288.04655355</v>
       </c>
     </row>
   </sheetData>

</xml_diff>